<commit_message>
Correções no verificador de dupla falta, agora será possivel melhorar o acumulador do Score e os dados para gera-lo
</commit_message>
<xml_diff>
--- a/Calculos simuladores.xlsx
+++ b/Calculos simuladores.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t xml:space="preserve">Serving Side</t>
   </si>
@@ -53,38 +53,41 @@
     <t xml:space="preserve">serving side</t>
   </si>
   <si>
+    <t xml:space="preserve">ball start</t>
+  </si>
+  <si>
     <t xml:space="preserve">ball side</t>
   </si>
   <si>
     <t xml:space="preserve">point place</t>
   </si>
   <si>
+    <t xml:space="preserve">De</t>
+  </si>
+  <si>
     <t xml:space="preserve">SS</t>
   </si>
   <si>
-    <t xml:space="preserve">De</t>
+    <t xml:space="preserve">Ad</t>
   </si>
   <si>
     <t xml:space="preserve">OS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,6 +109,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -195,60 +199,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -337,120 +337,120 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="2.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="n">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <f aca="false">D2-E2</f>
         <v>2</v>
       </c>
-      <c r="G2" s="0" t="str">
+      <c r="G2" s="1" t="str">
         <f aca="false">IF(F2&gt;0,$D$1,$E$1)</f>
         <v>A</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <f aca="false">COUNTIF($D$4:$D30, "AC")+COUNTIF($D$4:$D30, "FL")*2</f>
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="1" t="str">
+      <c r="G3" s="2" t="str">
         <f aca="false">IF($F$2&gt;0,"A", "B")</f>
         <v>A</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="str">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="str">
         <f aca="false">IF($F$2&gt;0,"B", "A")</f>
         <v>B</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="str">
+      <c r="A4" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A4)),"Ad", "Deuce"))</f>
         <v>Deuce</v>
       </c>
-      <c r="B4" s="5" t="str">
+      <c r="B4" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
-      <c r="C4" s="6" t="str">
+      <c r="C4" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C4)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C4, $D$1)+COUNTIF($C$4:$C4, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C4, $E$1)+COUNTIF($C$4:$C4, $D$1)&gt;0,"B","A")))</f>
         <v>A</v>
       </c>
-      <c r="D4" s="6" t="str">
+      <c r="D4" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", IF($C4=$B4,"AC","FL"))</f>
         <v>AC</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6" t="n">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C4,"A"),COUNTIF($C$4:$C4,"B")))</f>
         <v>1</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C4,"B"),COUNTIF($C$4:$C4,"A")))</f>
         <v>0</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="str">
+      <c r="A5" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A5)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A5)),"Ad", "Deuce"))</f>
         <v>Ad</v>
       </c>
-      <c r="B5" s="7" t="str">
+      <c r="B5" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A5)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
@@ -476,47 +476,47 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="str">
+      <c r="A6" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A6)),"Ad", "Deuce"))</f>
         <v>Deuce</v>
       </c>
-      <c r="B6" s="5" t="str">
+      <c r="B6" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
-      <c r="C6" s="6" t="str">
+      <c r="C6" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C6)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C6, $D$1)+COUNTIF($C$4:$C6, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C6, $E$1)+COUNTIF($C$4:$C6, $D$1)&gt;0,"B","A")))</f>
         <v>B</v>
       </c>
-      <c r="D6" s="6" t="str">
+      <c r="D6" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", IF($C6=$B6,"AC","FL"))</f>
         <v>FL</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6" t="n">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C6,"A"),COUNTIF($C$4:$C6,"B")))</f>
         <v>2</v>
       </c>
-      <c r="H6" s="6" t="str">
+      <c r="H6" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", "x")</f>
         <v>x</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I6" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C6,"B"),COUNTIF($C$4:$C6,"A")))</f>
         <v>1</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="str">
+      <c r="A7" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A7)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A7)),"Ad", "Deuce"))</f>
         <v>Ad</v>
       </c>
-      <c r="B7" s="7" t="str">
+      <c r="B7" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A7)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
@@ -542,47 +542,47 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="str">
+      <c r="A8" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A8)),"Ad", "Deuce"))</f>
         <v>Deuce</v>
       </c>
-      <c r="B8" s="5" t="str">
+      <c r="B8" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
-      <c r="C8" s="6" t="str">
+      <c r="C8" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C8)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C8, $D$1)+COUNTIF($C$4:$C8, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C8, $E$1)+COUNTIF($C$4:$C8, $D$1)&gt;0,"B","A")))</f>
         <v>B</v>
       </c>
-      <c r="D8" s="6" t="str">
+      <c r="D8" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", IF($C8=$B8,"AC","FL"))</f>
         <v>FL</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6" t="n">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C8,"A"),COUNTIF($C$4:$C8,"B")))</f>
         <v>3</v>
       </c>
-      <c r="H8" s="6" t="str">
+      <c r="H8" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", "x")</f>
         <v>x</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C8,"B"),COUNTIF($C$4:$C8,"A")))</f>
         <v>2</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="str">
+      <c r="A9" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A9)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A9)),"Ad", "Deuce"))</f>
         <v>Ad</v>
       </c>
-      <c r="B9" s="7" t="str">
+      <c r="B9" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A9)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
@@ -608,47 +608,47 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="str">
+      <c r="A10" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A10)),"Ad", "Deuce"))</f>
         <v>Deuce</v>
       </c>
-      <c r="B10" s="5" t="str">
+      <c r="B10" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
-      <c r="C10" s="6" t="str">
+      <c r="C10" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C10)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C10, $D$1)+COUNTIF($C$4:$C10, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C10, $E$1)+COUNTIF($C$4:$C10, $D$1)&gt;0,"B","A")))</f>
         <v>B</v>
       </c>
-      <c r="D10" s="6" t="str">
+      <c r="D10" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", IF($C10=$B10,"AC","FL"))</f>
         <v>FL</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6" t="n">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C10,"A"),COUNTIF($C$4:$C10,"B")))</f>
         <v>4</v>
       </c>
-      <c r="H10" s="6" t="str">
+      <c r="H10" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", "x")</f>
         <v>x</v>
       </c>
-      <c r="I10" s="6" t="n">
+      <c r="I10" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C10,"B"),COUNTIF($C$4:$C10,"A")))</f>
         <v>3</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="str">
+      <c r="A11" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A11)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A11)),"Ad", "Deuce"))</f>
         <v>Ad</v>
       </c>
-      <c r="B11" s="7" t="str">
+      <c r="B11" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A11)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
@@ -674,47 +674,47 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="str">
+      <c r="A12" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A12)),"Ad", "Deuce"))</f>
         <v>Deuce</v>
       </c>
-      <c r="B12" s="5" t="str">
+      <c r="B12" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
-      <c r="C12" s="6" t="str">
+      <c r="C12" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C12)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C12, $D$1)+COUNTIF($C$4:$C12, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C12, $E$1)+COUNTIF($C$4:$C12, $D$1)&gt;0,"B","A")))</f>
         <v>B</v>
       </c>
-      <c r="D12" s="6" t="str">
+      <c r="D12" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", IF($C12=$B12,"AC","FL"))</f>
         <v>FL</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6" t="n">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C12,"A"),COUNTIF($C$4:$C12,"B")))</f>
         <v>5</v>
       </c>
-      <c r="H12" s="6" t="str">
+      <c r="H12" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", "x")</f>
         <v>x</v>
       </c>
-      <c r="I12" s="6" t="n">
+      <c r="I12" s="7" t="n">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C12,"B"),COUNTIF($C$4:$C12,"A")))</f>
         <v>4</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="str">
+      <c r="A13" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A13)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A13)),"Ad", "Deuce"))</f>
         <v>Ad</v>
       </c>
-      <c r="B13" s="7" t="str">
+      <c r="B13" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A13)&gt; $D$2+$E$2, "", $A$2)</f>
         <v>A</v>
       </c>
@@ -740,47 +740,47 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="str">
+      <c r="A14" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A14)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B14" s="5" t="str">
+      <c r="B14" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
-      <c r="C14" s="6" t="str">
+      <c r="C14" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C14)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C14, $D$1)+COUNTIF($C$4:$C14, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C14, $E$1)+COUNTIF($C$4:$C14, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D14" s="6" t="str">
+      <c r="D14" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", IF($C14=$B14,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6" t="str">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C14,"A"),COUNTIF($C$4:$C14,"B")))</f>
         <v/>
       </c>
-      <c r="H14" s="6" t="str">
+      <c r="H14" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I14" s="6" t="str">
+      <c r="I14" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C14,"B"),COUNTIF($C$4:$C14,"A")))</f>
         <v/>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="str">
+      <c r="A15" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A15)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A15)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B15" s="7" t="str">
+      <c r="B15" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A15)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
@@ -806,47 +806,47 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="str">
+      <c r="A16" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A16)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B16" s="5" t="str">
+      <c r="B16" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
-      <c r="C16" s="6" t="str">
+      <c r="C16" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C16)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C16, $D$1)+COUNTIF($C$4:$C16, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C16, $E$1)+COUNTIF($C$4:$C16, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D16" s="6" t="str">
+      <c r="D16" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", IF($C16=$B16,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6" t="str">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C16,"A"),COUNTIF($C$4:$C16,"B")))</f>
         <v/>
       </c>
-      <c r="H16" s="6" t="str">
+      <c r="H16" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I16" s="6" t="str">
+      <c r="I16" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C16,"B"),COUNTIF($C$4:$C16,"A")))</f>
         <v/>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="str">
+      <c r="A17" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A17)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A17)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B17" s="7" t="str">
+      <c r="B17" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A17)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
@@ -872,47 +872,47 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="str">
+      <c r="A18" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A18)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B18" s="5" t="str">
+      <c r="B18" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
-      <c r="C18" s="6" t="str">
+      <c r="C18" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C18)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C18, $D$1)+COUNTIF($C$4:$C18, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C18, $E$1)+COUNTIF($C$4:$C18, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D18" s="6" t="str">
+      <c r="D18" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", IF($C18=$B18,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6" t="str">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C18,"A"),COUNTIF($C$4:$C18,"B")))</f>
         <v/>
       </c>
-      <c r="H18" s="6" t="str">
+      <c r="H18" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I18" s="6" t="str">
+      <c r="I18" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C18,"B"),COUNTIF($C$4:$C18,"A")))</f>
         <v/>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="str">
+      <c r="A19" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A19)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A19)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B19" s="7" t="str">
+      <c r="B19" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A19)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
@@ -938,47 +938,47 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="str">
+      <c r="A20" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A20)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B20" s="5" t="str">
+      <c r="B20" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
-      <c r="C20" s="6" t="str">
+      <c r="C20" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C20)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C20, $D$1)+COUNTIF($C$4:$C20, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C20, $E$1)+COUNTIF($C$4:$C20, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D20" s="6" t="str">
+      <c r="D20" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", IF($C20=$B20,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6" t="str">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C20,"A"),COUNTIF($C$4:$C20,"B")))</f>
         <v/>
       </c>
-      <c r="H20" s="6" t="str">
+      <c r="H20" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I20" s="6" t="str">
+      <c r="I20" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C20,"B"),COUNTIF($C$4:$C20,"A")))</f>
         <v/>
       </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="str">
+      <c r="A21" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A21)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A21)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B21" s="7" t="str">
+      <c r="B21" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A21)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
@@ -1004,47 +1004,47 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="str">
+      <c r="A22" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A22)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B22" s="5" t="str">
+      <c r="B22" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
-      <c r="C22" s="6" t="str">
+      <c r="C22" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C22)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C22, $D$1)+COUNTIF($C$4:$C22, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C22, $E$1)+COUNTIF($C$4:$C22, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D22" s="6" t="str">
+      <c r="D22" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", IF($C22=$B22,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6" t="str">
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C22,"A"),COUNTIF($C$4:$C22,"B")))</f>
         <v/>
       </c>
-      <c r="H22" s="6" t="str">
+      <c r="H22" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I22" s="6" t="str">
+      <c r="I22" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C22,"B"),COUNTIF($C$4:$C22,"A")))</f>
         <v/>
       </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="str">
+      <c r="A23" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A23)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A23)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B23" s="7" t="str">
+      <c r="B23" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A23)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
@@ -1070,47 +1070,47 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="str">
+      <c r="A24" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A24)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B24" s="5" t="str">
+      <c r="B24" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
-      <c r="C24" s="6" t="str">
+      <c r="C24" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C24)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C24, $D$1)+COUNTIF($C$4:$C24, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C24, $E$1)+COUNTIF($C$4:$C24, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D24" s="6" t="str">
+      <c r="D24" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", IF($C24=$B24,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="6" t="str">
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C24,"A"),COUNTIF($C$4:$C24,"B")))</f>
         <v/>
       </c>
-      <c r="H24" s="6" t="str">
+      <c r="H24" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I24" s="6" t="str">
+      <c r="I24" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C24,"B"),COUNTIF($C$4:$C24,"A")))</f>
         <v/>
       </c>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="str">
+      <c r="A25" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A25)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A25)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B25" s="7" t="str">
+      <c r="B25" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A25)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
@@ -1136,47 +1136,47 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="str">
+      <c r="A26" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A26)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B26" s="5" t="str">
+      <c r="B26" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
-      <c r="C26" s="6" t="str">
+      <c r="C26" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C26)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C26, $D$1)+COUNTIF($C$4:$C26, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C26, $E$1)+COUNTIF($C$4:$C26, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D26" s="6" t="str">
+      <c r="D26" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", IF($C26=$B26,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6" t="str">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C26,"A"),COUNTIF($C$4:$C26,"B")))</f>
         <v/>
       </c>
-      <c r="H26" s="6" t="str">
+      <c r="H26" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I26" s="6" t="str">
+      <c r="I26" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C26,"B"),COUNTIF($C$4:$C26,"A")))</f>
         <v/>
       </c>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="str">
+      <c r="A27" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A27)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A27)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B27" s="7" t="str">
+      <c r="B27" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A27)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
@@ -1202,47 +1202,47 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="str">
+      <c r="A28" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A28)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B28" s="5" t="str">
+      <c r="B28" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
-      <c r="C28" s="6" t="str">
+      <c r="C28" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C28)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C28, $D$1)+COUNTIF($C$4:$C28, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C28, $E$1)+COUNTIF($C$4:$C28, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D28" s="6" t="str">
+      <c r="D28" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", IF($C28=$B28,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="6" t="str">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C28,"A"),COUNTIF($C$4:$C28,"B")))</f>
         <v/>
       </c>
-      <c r="H28" s="6" t="str">
+      <c r="H28" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I28" s="6" t="str">
+      <c r="I28" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C28,"B"),COUNTIF($C$4:$C28,"A")))</f>
         <v/>
       </c>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="str">
+      <c r="A29" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A29)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A29)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B29" s="7" t="str">
+      <c r="B29" s="1" t="str">
         <f aca="false">IF(COUNTA($A$4:$A29)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
@@ -1268,40 +1268,40 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="str">
+      <c r="A30" s="5" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A30)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B30" s="5" t="str">
+      <c r="B30" s="6" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", $A$2)</f>
         <v/>
       </c>
-      <c r="C30" s="6" t="str">
+      <c r="C30" s="7" t="str">
         <f aca="false">IF(COUNTA($C$4:$C30)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C30, $D$1)+COUNTIF($C$4:$C30, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C30, $E$1)+COUNTIF($C$4:$C30, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D30" s="6" t="str">
+      <c r="D30" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", IF($C30=$B30,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="6" t="str">
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C30,"A"),COUNTIF($C$4:$C30,"B")))</f>
         <v/>
       </c>
-      <c r="H30" s="6" t="str">
+      <c r="H30" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I30" s="6" t="str">
+      <c r="I30" s="7" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C30,"B"),COUNTIF($C$4:$C30,"A")))</f>
         <v/>
       </c>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1319,96 +1319,99 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="6.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="7.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="6.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="2.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="D2" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <f aca="false">D2-E2</f>
         <v>6</v>
       </c>
-      <c r="G2" s="0" t="str">
+      <c r="G2" s="1" t="str">
         <f aca="false">IF(F2&gt;0,$D$1,$E$1)</f>
         <v>A</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <f aca="false">COUNTIF($D$4:$D30, "AC")+COUNTIF($D$4:$D30, "FL")*2</f>
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="1" t="str">
+      <c r="G3" s="2" t="str">
         <f aca="false">IF($F$2&gt;0,"A", "B")</f>
         <v>A</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="str">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="str">
         <f aca="false">IF($F$2&gt;0,"B", "A")</f>
         <v>B</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,49 +1419,48 @@
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A4)),"Ad", "Deuce"))</f>
         <v>Deuce</v>
       </c>
-      <c r="B4" s="10" t="str">
+      <c r="B4" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B4)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v>A</v>
       </c>
-      <c r="C4" s="10" t="str">
+      <c r="C4" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C4)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C4, $D$1)+COUNTIF($C$4:$C4, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C4, $E$1)+COUNTIF($C$4:$C4, $D$1)&gt;0,"B","A")))</f>
         <v>A</v>
       </c>
-      <c r="D4" s="10" t="str">
+      <c r="D4" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", IF($C4=$B4,"AC","FL"))</f>
         <v>AC</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10" t="n">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C4,"A"),COUNTIF($C$4:$C4,"B")))</f>
         <v>1</v>
       </c>
-      <c r="H4" s="10" t="str">
+      <c r="H4" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", "x")</f>
         <v>x</v>
       </c>
-      <c r="I4" s="10" t="n">
+      <c r="I4" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A4)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C4,"B"),COUNTIF($C$4:$C4,"A")))</f>
         <v>0</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>3</v>
-      </c>
+      <c r="L4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="str">
+      <c r="A5" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A5)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A5)),"Ad", "Deuce"))</f>
         <v>Ad</v>
       </c>
@@ -1474,10 +1476,6 @@
         <f aca="false">IF(COUNTA($A$4:$A5)&gt; $D$2+$E$2, "", IF($C5=$B5,"AC","FL"))</f>
         <v>FL</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="7"/>
       <c r="G5" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A5)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C5,"A"),COUNTIF($C$4:$C5,"B")))</f>
         <v>2</v>
@@ -1490,67 +1488,67 @@
         <f aca="false">IF(COUNTA($A$4:$A5)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C5,"B"),COUNTIF($C$4:$C5,"A")))</f>
         <v>0</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>3</v>
-      </c>
+      <c r="L5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A6)),"Ad", "Deuce"))</f>
         <v>Deuce</v>
       </c>
-      <c r="B6" s="10" t="str">
+      <c r="B6" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B6)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v>B</v>
       </c>
-      <c r="C6" s="10" t="str">
+      <c r="C6" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C6)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C6, $D$1)+COUNTIF($C$4:$C6, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C6, $E$1)+COUNTIF($C$4:$C6, $D$1)&gt;0,"B","A")))</f>
         <v>A</v>
       </c>
-      <c r="D6" s="10" t="str">
+      <c r="D6" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", IF($C6=$B6,"AC","FL"))</f>
         <v>FL</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10" t="n">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C6,"A"),COUNTIF($C$4:$C6,"B")))</f>
         <v>3</v>
       </c>
-      <c r="H6" s="10" t="str">
+      <c r="H6" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", "x")</f>
         <v>x</v>
       </c>
-      <c r="I6" s="10" t="n">
+      <c r="I6" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A6)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C6,"B"),COUNTIF($C$4:$C6,"A")))</f>
         <v>0</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>3</v>
-      </c>
+      <c r="L6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="str">
+      <c r="A7" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A7)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A7)),"Ad", "Deuce"))</f>
         <v>Ad</v>
       </c>
@@ -1566,10 +1564,6 @@
         <f aca="false">IF(COUNTA($A$4:$A7)&gt; $D$2+$E$2, "", IF($C7=$B7,"AC","FL"))</f>
         <v>AC</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="7"/>
       <c r="G7" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A7)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C7,"A"),COUNTIF($C$4:$C7,"B")))</f>
         <v>4</v>
@@ -1582,67 +1576,67 @@
         <f aca="false">IF(COUNTA($A$4:$A7)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C7,"B"),COUNTIF($C$4:$C7,"A")))</f>
         <v>0</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>3</v>
-      </c>
+      <c r="L7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A8)),"Ad", "Deuce"))</f>
         <v>Deuce</v>
       </c>
-      <c r="B8" s="10" t="str">
+      <c r="B8" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B8)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v>A</v>
       </c>
-      <c r="C8" s="10" t="str">
+      <c r="C8" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C8)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C8, $D$1)+COUNTIF($C$4:$C8, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C8, $E$1)+COUNTIF($C$4:$C8, $D$1)&gt;0,"B","A")))</f>
         <v>A</v>
       </c>
-      <c r="D8" s="10" t="str">
+      <c r="D8" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", IF($C8=$B8,"AC","FL"))</f>
         <v>AC</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10" t="n">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C8,"A"),COUNTIF($C$4:$C8,"B")))</f>
         <v>5</v>
       </c>
-      <c r="H8" s="10" t="str">
+      <c r="H8" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", "x")</f>
         <v>x</v>
       </c>
-      <c r="I8" s="10" t="n">
+      <c r="I8" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A8)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C8,"B"),COUNTIF($C$4:$C8,"A")))</f>
         <v>0</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>3</v>
-      </c>
+      <c r="L8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="str">
+      <c r="A9" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A9)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A9)),"Ad", "Deuce"))</f>
         <v>Ad</v>
       </c>
@@ -1658,10 +1652,6 @@
         <f aca="false">IF(COUNTA($A$4:$A9)&gt; $D$2+$E$2, "", IF($C9=$B9,"AC","FL"))</f>
         <v>FL</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="7"/>
       <c r="G9" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A9)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C9,"A"),COUNTIF($C$4:$C9,"B")))</f>
         <v>6</v>
@@ -1674,67 +1664,67 @@
         <f aca="false">IF(COUNTA($A$4:$A9)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C9,"B"),COUNTIF($C$4:$C9,"A")))</f>
         <v>0</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>3</v>
-      </c>
+      <c r="L9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A10)),"Ad", "Deuce"))</f>
         <v>Deuce</v>
       </c>
-      <c r="B10" s="10" t="str">
+      <c r="B10" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B10)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v>B</v>
       </c>
-      <c r="C10" s="10" t="str">
+      <c r="C10" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C10)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C10, $D$1)+COUNTIF($C$4:$C10, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C10, $E$1)+COUNTIF($C$4:$C10, $D$1)&gt;0,"B","A")))</f>
         <v>B</v>
       </c>
-      <c r="D10" s="10" t="str">
+      <c r="D10" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", IF($C10=$B10,"AC","FL"))</f>
         <v>AC</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10" t="n">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C10,"A"),COUNTIF($C$4:$C10,"B")))</f>
         <v>6</v>
       </c>
-      <c r="H10" s="10" t="str">
+      <c r="H10" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", "x")</f>
         <v>x</v>
       </c>
-      <c r="I10" s="10" t="n">
+      <c r="I10" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A10)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C10,"B"),COUNTIF($C$4:$C10,"A")))</f>
         <v>1</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="L10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="str">
+      <c r="A11" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A11)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A11)),"Ad", "Deuce"))</f>
         <v>Ad</v>
       </c>
@@ -1750,10 +1740,6 @@
         <f aca="false">IF(COUNTA($A$4:$A11)&gt; $D$2+$E$2, "", IF($C11=$B11,"AC","FL"))</f>
         <v>AC</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="7"/>
       <c r="G11" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A11)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C11,"A"),COUNTIF($C$4:$C11,"B")))</f>
         <v>7</v>
@@ -1766,310 +1752,261 @@
         <f aca="false">IF(COUNTA($A$4:$A11)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C11,"B"),COUNTIF($C$4:$C11,"A")))</f>
         <v>1</v>
       </c>
-      <c r="J11" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>3</v>
-      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A12)),"Ad", "Deuce"))</f>
-        <v/>
-      </c>
-      <c r="B12" s="10" t="str">
+        <v>Deuce</v>
+      </c>
+      <c r="B12" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B12)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
-        <v/>
-      </c>
-      <c r="C12" s="10" t="str">
+        <v>A</v>
+      </c>
+      <c r="C12" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C12)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C12, $D$1)+COUNTIF($C$4:$C12, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C12, $E$1)+COUNTIF($C$4:$C12, $D$1)&gt;0,"B","A")))</f>
-        <v/>
-      </c>
-      <c r="D12" s="10" t="str">
+        <v>B</v>
+      </c>
+      <c r="D12" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", IF($C12=$B12,"AC","FL"))</f>
-        <v/>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10" t="str">
+        <v>FL</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C12,"A"),COUNTIF($C$4:$C12,"B")))</f>
-        <v/>
-      </c>
-      <c r="H12" s="10" t="str">
+        <v>7</v>
+      </c>
+      <c r="H12" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", "x")</f>
-        <v/>
-      </c>
-      <c r="I12" s="10" t="str">
+        <v>x</v>
+      </c>
+      <c r="I12" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A12)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C12,"B"),COUNTIF($C$4:$C12,"A")))</f>
-        <v/>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="str">
+      <c r="A13" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A13)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A13)),"Ad", "Deuce"))</f>
-        <v/>
+        <v>Ad</v>
       </c>
       <c r="B13" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A13)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B13)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
-        <v/>
+        <v>B</v>
       </c>
       <c r="C13" s="8" t="str">
         <f aca="false">IF(COUNTA($C$4:$C13)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C13, $D$1)+COUNTIF($C$4:$C13, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C13, $E$1)+COUNTIF($C$4:$C13, $D$1)&gt;0,"B","A")))</f>
-        <v/>
+        <v>A</v>
       </c>
       <c r="D13" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A13)&gt; $D$2+$E$2, "", IF($C13=$B13,"AC","FL"))</f>
-        <v/>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8" t="str">
+        <v>FL</v>
+      </c>
+      <c r="G13" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A13)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C13,"A"),COUNTIF($C$4:$C13,"B")))</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="H13" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A13)&gt; $D$2+$E$2, "", "x")</f>
-        <v/>
-      </c>
-      <c r="I13" s="8" t="str">
+        <v>x</v>
+      </c>
+      <c r="I13" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A13)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C13,"B"),COUNTIF($C$4:$C13,"A")))</f>
-        <v/>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A14)),"Ad", "Deuce"))</f>
-        <v/>
-      </c>
-      <c r="B14" s="10" t="str">
+        <v>Deuce</v>
+      </c>
+      <c r="B14" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B14)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
-        <v/>
-      </c>
-      <c r="C14" s="10" t="str">
+        <v>B</v>
+      </c>
+      <c r="C14" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C14)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C14, $D$1)+COUNTIF($C$4:$C14, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C14, $E$1)+COUNTIF($C$4:$C14, $D$1)&gt;0,"B","A")))</f>
-        <v/>
-      </c>
-      <c r="D14" s="10" t="str">
+        <v>B</v>
+      </c>
+      <c r="D14" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", IF($C14=$B14,"AC","FL"))</f>
-        <v/>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10" t="str">
+        <v>AC</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C14,"A"),COUNTIF($C$4:$C14,"B")))</f>
-        <v/>
-      </c>
-      <c r="H14" s="10" t="str">
+        <v>8</v>
+      </c>
+      <c r="H14" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", "x")</f>
-        <v/>
-      </c>
-      <c r="I14" s="10" t="str">
+        <v>x</v>
+      </c>
+      <c r="I14" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A14)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C14,"B"),COUNTIF($C$4:$C14,"A")))</f>
-        <v/>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="str">
+      <c r="A15" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A15)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A15)),"Ad", "Deuce"))</f>
-        <v/>
+        <v>Ad</v>
       </c>
       <c r="B15" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A15)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B15)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
-        <v/>
+        <v>A</v>
       </c>
       <c r="C15" s="8" t="str">
         <f aca="false">IF(COUNTA($C$4:$C15)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C15, $D$1)+COUNTIF($C$4:$C15, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C15, $E$1)+COUNTIF($C$4:$C15, $D$1)&gt;0,"B","A")))</f>
-        <v/>
+        <v>A</v>
       </c>
       <c r="D15" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A15)&gt; $D$2+$E$2, "", IF($C15=$B15,"AC","FL"))</f>
-        <v/>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8" t="str">
+        <v>AC</v>
+      </c>
+      <c r="G15" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A15)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C15,"A"),COUNTIF($C$4:$C15,"B")))</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="H15" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A15)&gt; $D$2+$E$2, "", "x")</f>
-        <v/>
-      </c>
-      <c r="I15" s="8" t="str">
+        <v>x</v>
+      </c>
+      <c r="I15" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A15)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C15,"B"),COUNTIF($C$4:$C15,"A")))</f>
-        <v/>
-      </c>
-      <c r="J15" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="K15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="13" t="s">
-        <v>3</v>
-      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A16)),"Ad", "Deuce"))</f>
-        <v/>
-      </c>
-      <c r="B16" s="10" t="str">
+        <v>Deuce</v>
+      </c>
+      <c r="B16" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B16)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
-        <v/>
-      </c>
-      <c r="C16" s="10" t="str">
+        <v>A</v>
+      </c>
+      <c r="C16" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C16)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C16, $D$1)+COUNTIF($C$4:$C16, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C16, $E$1)+COUNTIF($C$4:$C16, $D$1)&gt;0,"B","A")))</f>
-        <v/>
-      </c>
-      <c r="D16" s="10" t="str">
+        <v>B</v>
+      </c>
+      <c r="D16" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", IF($C16=$B16,"AC","FL"))</f>
-        <v/>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="10" t="str">
+        <v>FL</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C16,"A"),COUNTIF($C$4:$C16,"B")))</f>
-        <v/>
-      </c>
-      <c r="H16" s="10" t="str">
+        <v>9</v>
+      </c>
+      <c r="H16" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", "x")</f>
-        <v/>
-      </c>
-      <c r="I16" s="10" t="str">
+        <v>x</v>
+      </c>
+      <c r="I16" s="9" t="n">
         <f aca="false">IF(COUNTA($A$4:$A16)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C16,"B"),COUNTIF($C$4:$C16,"A")))</f>
-        <v/>
-      </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="12"/>
+        <v>4</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="str">
+      <c r="A17" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A17)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A17)),"Ad", "Deuce"))</f>
-        <v/>
+        <v>Ad</v>
       </c>
       <c r="B17" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A17)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B17)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
-        <v/>
+        <v>B</v>
       </c>
       <c r="C17" s="8" t="str">
         <f aca="false">IF(COUNTA($C$4:$C17)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C17, $D$1)+COUNTIF($C$4:$C17, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C17, $E$1)+COUNTIF($C$4:$C17, $D$1)&gt;0,"B","A")))</f>
-        <v/>
+        <v>A</v>
       </c>
       <c r="D17" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A17)&gt; $D$2+$E$2, "", IF($C17=$B17,"AC","FL"))</f>
-        <v/>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8" t="str">
+        <v>FL</v>
+      </c>
+      <c r="G17" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A17)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C17,"A"),COUNTIF($C$4:$C17,"B")))</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="H17" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A17)&gt; $D$2+$E$2, "", "x")</f>
-        <v/>
-      </c>
-      <c r="I17" s="8" t="str">
+        <v>x</v>
+      </c>
+      <c r="I17" s="8" t="n">
         <f aca="false">IF(COUNTA($A$4:$A17)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C17,"B"),COUNTIF($C$4:$C17,"A")))</f>
-        <v/>
-      </c>
-      <c r="M17" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A18)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B18" s="10" t="str">
+      <c r="B18" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B18)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v/>
       </c>
-      <c r="C18" s="10" t="str">
+      <c r="C18" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C18)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C18, $D$1)+COUNTIF($C$4:$C18, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C18, $E$1)+COUNTIF($C$4:$C18, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D18" s="10" t="str">
+      <c r="D18" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", IF($C18=$B18,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="10" t="str">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C18,"A"),COUNTIF($C$4:$C18,"B")))</f>
         <v/>
       </c>
-      <c r="H18" s="10" t="str">
+      <c r="H18" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I18" s="10" t="str">
+      <c r="I18" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A18)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C18,"B"),COUNTIF($C$4:$C18,"A")))</f>
         <v/>
       </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="12"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="str">
+      <c r="A19" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A19)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A19)),"Ad", "Deuce"))</f>
         <v/>
       </c>
@@ -2085,8 +2022,6 @@
         <f aca="false">IF(COUNTA($A$4:$A19)&gt; $D$2+$E$2, "", IF($C19=$B19,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
       <c r="G19" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A19)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C19,"A"),COUNTIF($C$4:$C19,"B")))</f>
         <v/>
@@ -2099,46 +2034,46 @@
         <f aca="false">IF(COUNTA($A$4:$A19)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C19,"B"),COUNTIF($C$4:$C19,"A")))</f>
         <v/>
       </c>
-      <c r="M19" s="13"/>
+      <c r="M19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A20)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B20" s="10" t="str">
+      <c r="B20" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B20)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v/>
       </c>
-      <c r="C20" s="10" t="str">
+      <c r="C20" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C20)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C20, $D$1)+COUNTIF($C$4:$C20, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C20, $E$1)+COUNTIF($C$4:$C20, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D20" s="10" t="str">
+      <c r="D20" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", IF($C20=$B20,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="10" t="str">
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C20,"A"),COUNTIF($C$4:$C20,"B")))</f>
         <v/>
       </c>
-      <c r="H20" s="10" t="str">
+      <c r="H20" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I20" s="10" t="str">
+      <c r="I20" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A20)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C20,"B"),COUNTIF($C$4:$C20,"A")))</f>
         <v/>
       </c>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="12"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="str">
+      <c r="A21" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A21)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A21)),"Ad", "Deuce"))</f>
         <v/>
       </c>
@@ -2154,8 +2089,6 @@
         <f aca="false">IF(COUNTA($A$4:$A21)&gt; $D$2+$E$2, "", IF($C21=$B21,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
       <c r="G21" s="8" t="str">
         <f aca="false">IF(COUNTA($A$4:$A21)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C21,"A"),COUNTIF($C$4:$C21,"B")))</f>
         <v/>
@@ -2168,46 +2101,46 @@
         <f aca="false">IF(COUNTA($A$4:$A21)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C21,"B"),COUNTIF($C$4:$C21,"A")))</f>
         <v/>
       </c>
-      <c r="M21" s="13"/>
+      <c r="M21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A22)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B22" s="10" t="str">
+      <c r="B22" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B22)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v/>
       </c>
-      <c r="C22" s="10" t="str">
+      <c r="C22" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C22)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C22, $D$1)+COUNTIF($C$4:$C22, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C22, $E$1)+COUNTIF($C$4:$C22, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D22" s="10" t="str">
+      <c r="D22" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", IF($C22=$B22,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="10" t="str">
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C22,"A"),COUNTIF($C$4:$C22,"B")))</f>
         <v/>
       </c>
-      <c r="H22" s="10" t="str">
+      <c r="H22" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I22" s="10" t="str">
+      <c r="I22" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A22)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C22,"B"),COUNTIF($C$4:$C22,"A")))</f>
         <v/>
       </c>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="12"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="str">
+      <c r="A23" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A23)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A23)),"Ad", "Deuce"))</f>
         <v/>
       </c>
@@ -2235,46 +2168,46 @@
         <f aca="false">IF(COUNTA($A$4:$A23)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C23,"B"),COUNTIF($C$4:$C23,"A")))</f>
         <v/>
       </c>
-      <c r="M23" s="13"/>
+      <c r="M23" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A24)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B24" s="10" t="str">
+      <c r="B24" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B24)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v/>
       </c>
-      <c r="C24" s="10" t="str">
+      <c r="C24" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C24)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C24, $D$1)+COUNTIF($C$4:$C24, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C24, $E$1)+COUNTIF($C$4:$C24, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D24" s="10" t="str">
+      <c r="D24" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", IF($C24=$B24,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="10" t="str">
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C24,"A"),COUNTIF($C$4:$C24,"B")))</f>
         <v/>
       </c>
-      <c r="H24" s="10" t="str">
+      <c r="H24" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I24" s="10" t="str">
+      <c r="I24" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A24)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C24,"B"),COUNTIF($C$4:$C24,"A")))</f>
         <v/>
       </c>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="12"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="str">
+      <c r="A25" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A25)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A25)),"Ad", "Deuce"))</f>
         <v/>
       </c>
@@ -2302,46 +2235,46 @@
         <f aca="false">IF(COUNTA($A$4:$A25)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C25,"B"),COUNTIF($C$4:$C25,"A")))</f>
         <v/>
       </c>
-      <c r="M25" s="13"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A26)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B26" s="10" t="str">
+      <c r="B26" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B26)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v/>
       </c>
-      <c r="C26" s="10" t="str">
+      <c r="C26" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C26)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C26, $D$1)+COUNTIF($C$4:$C26, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C26, $E$1)+COUNTIF($C$4:$C26, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D26" s="10" t="str">
+      <c r="D26" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", IF($C26=$B26,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="10" t="str">
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C26,"A"),COUNTIF($C$4:$C26,"B")))</f>
         <v/>
       </c>
-      <c r="H26" s="10" t="str">
+      <c r="H26" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I26" s="10" t="str">
+      <c r="I26" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A26)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C26,"B"),COUNTIF($C$4:$C26,"A")))</f>
         <v/>
       </c>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="12"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="str">
+      <c r="A27" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A27)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A27)),"Ad", "Deuce"))</f>
         <v/>
       </c>
@@ -2369,46 +2302,46 @@
         <f aca="false">IF(COUNTA($A$4:$A27)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C27,"B"),COUNTIF($C$4:$C27,"A")))</f>
         <v/>
       </c>
-      <c r="M27" s="13"/>
+      <c r="M27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A28)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B28" s="10" t="str">
+      <c r="B28" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B28)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v/>
       </c>
-      <c r="C28" s="10" t="str">
+      <c r="C28" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C28)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C28, $D$1)+COUNTIF($C$4:$C28, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C28, $E$1)+COUNTIF($C$4:$C28, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D28" s="10" t="str">
+      <c r="D28" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", IF($C28=$B28,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="10" t="str">
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C28,"A"),COUNTIF($C$4:$C28,"B")))</f>
         <v/>
       </c>
-      <c r="H28" s="10" t="str">
+      <c r="H28" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I28" s="10" t="str">
+      <c r="I28" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A28)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C28,"B"),COUNTIF($C$4:$C28,"A")))</f>
         <v/>
       </c>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="12"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="str">
+      <c r="A29" s="4" t="str">
         <f aca="false">IF(COUNTA($A$4:$A29)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A29)),"Ad", "Deuce"))</f>
         <v/>
       </c>
@@ -2436,43 +2369,43 @@
         <f aca="false">IF(COUNTA($A$4:$A29)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C29,"B"),COUNTIF($C$4:$C29,"A")))</f>
         <v/>
       </c>
-      <c r="M29" s="13"/>
+      <c r="M29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", IF(ISEVEN(COUNTA($A$4:$A30)),"Ad", "Deuce"))</f>
         <v/>
       </c>
-      <c r="B30" s="10" t="str">
+      <c r="B30" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", IF(ISEVEN(ROUND((COUNTA($B$4:$B30)+1)/2,0)), IF($A$2 = "A", "B", "A"), IF($A$2 = "A", "A", "B")))</f>
         <v/>
       </c>
-      <c r="C30" s="10" t="str">
+      <c r="C30" s="9" t="str">
         <f aca="false">IF(COUNTA($C$4:$C30)&gt; $D$2+$E$2, "",IF($F$2&gt;0, IF(ABS($F$2)-COUNTIF($C$4:$C30, $D$1)+COUNTIF($C$4:$C30, $E$1)&gt;0,"A","B"),IF(ABS($F$2)-COUNTIF($C$4:$C30, $E$1)+COUNTIF($C$4:$C30, $D$1)&gt;0,"B","A")))</f>
         <v/>
       </c>
-      <c r="D30" s="10" t="str">
+      <c r="D30" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", IF($C30=$B30,"AC","FL"))</f>
         <v/>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="10" t="str">
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C30,"A"),COUNTIF($C$4:$C30,"B")))</f>
         <v/>
       </c>
-      <c r="H30" s="10" t="str">
+      <c r="H30" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", "x")</f>
         <v/>
       </c>
-      <c r="I30" s="10" t="str">
+      <c r="I30" s="9" t="str">
         <f aca="false">IF(COUNTA($A$4:$A30)&gt; $D$2+$E$2, "", IF($F$2&gt;0,COUNTIF($C$4:$C30,"B"),COUNTIF($C$4:$C30,"A")))</f>
         <v/>
       </c>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="12"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>